<commit_message>
New version of Excel Sheet
</commit_message>
<xml_diff>
--- a/ESP32.xlsx
+++ b/ESP32.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="244">
   <si>
     <t>ESP32</t>
   </si>
@@ -758,6 +758,9 @@
   </si>
   <si>
     <t>ADC1_CH04</t>
+  </si>
+  <si>
+    <t>UNUSABLE !!! (Flash memory)</t>
   </si>
 </sst>
 </file>
@@ -788,12 +791,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -808,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -823,11 +832,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1335,7 +1345,7 @@
   <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:D33"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,161 +1590,216 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="9">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4" t="s">
+      <c r="E8" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="M8" s="9"/>
+      <c r="N8" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="O8" s="9"/>
+      <c r="P8" s="9" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="9">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4" t="s">
+      <c r="E9" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="L9" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="M9" s="9"/>
+      <c r="N9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="O9" s="9"/>
+      <c r="P9" s="9" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="9">
         <v>22</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4" t="s">
+      <c r="E10" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="M10" s="9"/>
+      <c r="N10" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="O10" s="9"/>
+      <c r="P10" s="9" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="9">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4" t="s">
+      <c r="E11" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="M11" s="9"/>
+      <c r="N11" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="O11" s="9"/>
+      <c r="P11" s="9" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="9">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4" t="s">
+      <c r="E12" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="M12" s="9"/>
+      <c r="N12" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="O12" s="9"/>
+      <c r="P12" s="9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="9">
         <v>19</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="C13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4" t="s">
+      <c r="E13" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2341,31 +2406,31 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F44" s="8"/>
+      <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F45" s="7"/>
+      <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F46" s="7"/>
+      <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F47" s="7"/>
+      <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="F48" s="7"/>
+      <c r="F48" s="8"/>
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
     </row>
     <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="7"/>
+      <c r="F49" s="8"/>
     </row>
     <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="7"/>
+      <c r="F50" s="8"/>
     </row>
   </sheetData>
-  <sortState ref="A2:T56">
-    <sortCondition ref="D2:D56"/>
+  <sortState ref="A2:Y50">
+    <sortCondition ref="D2:D50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>